<commit_message>
Minor changes to spacing
</commit_message>
<xml_diff>
--- a/results/GAM/GAM_results.xlsx
+++ b/results/GAM/GAM_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Thesis\Data analysis\Individual Species Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ORnearshore_groundfish\results\GAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3C44DB-57FF-49CF-A407-340CDC4698BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3608232F-46EA-4FF1-A050-030CF6745EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{AE5C508A-1220-480B-9FC8-22A5998BFD8B}"/>
+    <workbookView xWindow="-28920" yWindow="-6750" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{AE5C508A-1220-480B-9FC8-22A5998BFD8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Petrale" sheetId="2" r:id="rId1"/>
@@ -3913,7 +3913,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4158,7 +4158,7 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="6">
@@ -4228,7 +4228,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="6">
@@ -4245,7 +4245,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="6">

</xml_diff>